<commit_message>
Last updates before sending to CDMO.  Everything works locally.
</commit_message>
<xml_diff>
--- a/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_HEE_2020.xlsx
+++ b/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_HEE_2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Global_Decisions--&gt;" sheetId="1" state="visible" r:id="rId2"/>
@@ -459,7 +459,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -467,6 +467,10 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -492,10 +496,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="1" sqref="E2:E13 C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -515,14 +519,14 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="E2:E13 A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="1" max="1" min="1" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="2" style="0" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="0" width="22.01"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="1" max="1" min="1" style="2" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="2" style="2" width="19.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="2" width="22.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -768,10 +772,10 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="E2:E13 A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -799,7 +803,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -822,12 +826,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+      <selection pane="topLeft" activeCell="G34" activeCellId="1" sqref="E2:E13 G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="2" style="0" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="2" style="2" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -869,23 +873,23 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="1" style="0" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="3" min="3" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="5" min="4" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="9" min="8" style="0" width="8.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="10" min="10" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="11" min="11" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="12" min="12" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="13" min="13" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="14" min="14" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="1" style="2" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="3" min="3" style="2" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="5" min="4" style="2" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="2" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="2" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="9" min="8" style="2" width="8.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="10" min="10" style="2" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="11" min="11" style="2" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="12" min="12" style="2" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="13" min="13" style="2" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="14" min="14" style="2" width="12.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -918,6 +922,7 @@
       <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
@@ -932,6 +937,7 @@
       <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
@@ -946,6 +952,7 @@
       <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
@@ -960,6 +967,7 @@
       <c r="B5" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
@@ -974,6 +982,7 @@
       <c r="B6" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
@@ -988,6 +997,7 @@
       <c r="B7" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1002,6 +1012,7 @@
       <c r="B8" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1016,6 +1027,7 @@
       <c r="B9" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1030,6 +1042,7 @@
       <c r="B10" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1044,6 +1057,7 @@
       <c r="B11" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1058,6 +1072,7 @@
       <c r="B12" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1072,6 +1087,7 @@
       <c r="B13" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1106,34 +1122,34 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="E2:E13 C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="1" style="0" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="3" min="3" style="0" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="4" min="4" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="5" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="1" style="2" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="3" min="3" style="2" width="18.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="4" min="4" style="2" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="5" style="2" width="18.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1144,16 +1160,16 @@
       <c r="B2" s="1" t="n">
         <v>-157.8333</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1164,13 +1180,13 @@
       <c r="B3" s="1" t="n">
         <v>21.4075</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1181,13 +1197,13 @@
       <c r="B4" s="1" t="n">
         <v>-157.7771</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1198,7 +1214,7 @@
       <c r="B5" s="1" t="n">
         <v>21.4628</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1221,13 +1237,13 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="E2:E13 A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="1" min="1" style="0" width="49.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="1" min="1" style="2" width="49.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1319,10 +1335,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1345,10 +1361,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
+      <selection pane="topLeft" activeCell="G33" activeCellId="1" sqref="E2:E13 G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1368,17 +1384,17 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="E2:E13 A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="1" max="1" min="1" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="2" style="0" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="4" min="3" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="5" min="5" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="0" width="28.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="1" max="1" min="1" style="2" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="2" style="2" width="19.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="4" min="3" style="2" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="5" min="5" style="2" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="2" width="31.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="2" width="28.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1397,7 +1413,7 @@
       <c r="E1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1414,7 +1430,7 @@
       <c r="D2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1431,7 +1447,7 @@
       <c r="D3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1451,7 +1467,7 @@
       <c r="E4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1468,7 +1484,7 @@
       <c r="D5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1485,7 +1501,7 @@
       <c r="D6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1502,7 +1518,7 @@
       <c r="D7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1519,7 +1535,7 @@
       <c r="D8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1536,7 +1552,7 @@
       <c r="D9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1553,7 +1569,7 @@
       <c r="D10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1570,7 +1586,7 @@
       <c r="D11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1587,7 +1603,7 @@
       <c r="D12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1604,7 +1620,7 @@
       <c r="D13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1621,7 +1637,7 @@
       <c r="D14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1638,7 +1654,7 @@
       <c r="D15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1655,7 +1671,7 @@
       <c r="D16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1672,7 +1688,7 @@
       <c r="D17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1689,7 +1705,7 @@
       <c r="D18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1706,7 +1722,7 @@
       <c r="D19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1723,7 +1739,7 @@
       <c r="D20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1740,7 +1756,7 @@
       <c r="D21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1757,7 +1773,7 @@
       <c r="D22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1779,19 +1795,19 @@
   </sheetPr>
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N15" activeCellId="1" sqref="E2:E13 N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.3359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="1" max="1" min="1" style="0" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="2" style="0" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="3" min="3" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="11" min="6" style="0" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="12" min="12" style="0" width="16.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="13" min="13" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="14" min="14" style="0" width="10"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="1" max="1" min="1" style="2" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="2" min="2" style="2" width="19.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="3" min="3" style="2" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="11" min="6" style="2" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="12" min="12" style="2" width="16.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="13" min="13" style="2" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="14" min="14" style="2" width="10"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2139,7 +2155,7 @@
         <v>106</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="M15" s="1" t="n">
         <v>0.015</v>
@@ -2260,7 +2276,7 @@
         <v>106</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="M20" s="1" t="n">
         <v>6</v>
@@ -2321,7 +2337,7 @@
         <v>106</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="M22" s="1" t="n">
         <v>0.015</v>

</xml_diff>